<commit_message>
Step 1 - quiz automation csv to json - one question
</commit_message>
<xml_diff>
--- a/quizapp/src/tools/12th_Bio_Botany_Tamil_U02_01.xlsx
+++ b/quizapp/src/tools/12th_Bio_Botany_Tamil_U02_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2020\git\quiz_app\quizapp\src\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37DB84F-54D7-4BD1-A389-840ECE9E3ED2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9059E923-6517-449C-AB0E-D2045CA647F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -562,7 +562,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -579,7 +581,7 @@
     <col min="13" max="16384" width="10.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>